<commit_message>
new password is added
</commit_message>
<xml_diff>
--- a/tables.xlsx
+++ b/tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\egeok\Desktop\database\itucsdb1938\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7188075-CD88-4E3B-9900-0991B4078F12}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C73DE35D-91BF-4D9C-BB03-916647C82F01}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17490" windowHeight="7980" xr2:uid="{CD6D5736-004C-459B-A721-EBD61DD79355}"/>
   </bookViews>
@@ -258,13 +258,13 @@
     <t>Provider Company Name</t>
   </si>
   <si>
-    <t>Supply Order ID</t>
-  </si>
-  <si>
     <t>Time</t>
   </si>
   <si>
     <t>Product Name</t>
+  </si>
+  <si>
+    <t>Supply Order ID(key)</t>
   </si>
 </sst>
 </file>
@@ -631,8 +631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{157BF2EA-2308-4D4D-BD43-7AC7134C789C}">
   <dimension ref="A2:P24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -980,7 +980,7 @@
         <v>70</v>
       </c>
       <c r="B20" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C20" t="s">
         <v>69</v>
@@ -992,10 +992,10 @@
         <v>3</v>
       </c>
       <c r="F20" t="s">
+        <v>77</v>
+      </c>
+      <c r="G20" t="s">
         <v>78</v>
-      </c>
-      <c r="G20" t="s">
-        <v>79</v>
       </c>
       <c r="H20" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
added employee, cargocompany, marketplace tables
</commit_message>
<xml_diff>
--- a/tables.xlsx
+++ b/tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\egeok\Desktop\database\itucsdb1938\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C73DE35D-91BF-4D9C-BB03-916647C82F01}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F58C810C-0FBD-4E0D-83AD-D331E5F22C07}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17490" windowHeight="7980" xr2:uid="{CD6D5736-004C-459B-A721-EBD61DD79355}"/>
   </bookViews>
@@ -288,12 +288,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -309,11 +315,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -632,7 +639,7 @@
   <dimension ref="A2:P24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="A8" sqref="A8:H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -742,28 +749,28 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="4" t="s">
         <v>19</v>
       </c>
     </row>
@@ -791,28 +798,28 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="4" t="s">
         <v>45</v>
       </c>
     </row>
@@ -872,48 +879,48 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" s="4" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G14" s="4" t="s">
         <v>75</v>
       </c>
     </row>

</xml_diff>